<commit_message>
analysis the source code
</commit_message>
<xml_diff>
--- a/Capstone time management.xlsx
+++ b/Capstone time management.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Thing I did</t>
   </si>
@@ -62,7 +62,13 @@
     <t>learn subversion</t>
   </si>
   <si>
-    <t>do some change</t>
+    <t>create repository for capstone</t>
+  </si>
+  <si>
+    <t>Get google source code</t>
+  </si>
+  <si>
+    <t>Extract Source code</t>
   </si>
 </sst>
 </file>
@@ -111,10 +117,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -427,7 +434,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,32 +518,62 @@
         <v>0.44861111111111113</v>
       </c>
       <c r="C4" s="2">
-        <v>0.875</v>
+        <v>0.53194444444444444</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" si="0"/>
-        <v>0.42638888888888887</v>
+        <v>8.3333333333333315E-2</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
       <c r="F5" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.9444444444444198E-3</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.625</v>
+      </c>
       <c r="F6" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.333333333333337E-2</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.875</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
able to pool data out
</commit_message>
<xml_diff>
--- a/Capstone time management.xlsx
+++ b/Capstone time management.xlsx
@@ -443,7 +443,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,100 +631,52 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F11" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F13" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F16" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="F16" s="2"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="F17" s="2"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F18" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="F18" s="2"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F19" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="F19" s="2"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="F20" s="2"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F21" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="F21" s="2"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F22" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="F22" s="2"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F23" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="F23" s="2"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F24" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="F24" s="2"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F25" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="F25" s="2"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F26" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="F26" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>